<commit_message>
Solo Project: ORM setup
</commit_message>
<xml_diff>
--- a/solo-project.xlsx
+++ b/solo-project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tiffany\coding-dojo\projects_and_algos\solo-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806DD203-B903-4CFE-80A4-91F39DE74C9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A869CA71-37BC-43B6-8C16-C24263B0AD36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overview" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Recipes and Grocery List App</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>User Dashboard</t>
-  </si>
-  <si>
-    <t>Perti-fy</t>
   </si>
   <si>
     <t>Refine</t>
@@ -188,6 +185,18 @@
   </si>
   <si>
     <t>Delete Recipe (R Book and Modify R)</t>
+  </si>
+  <si>
+    <t>ORM Database (Alt)</t>
+  </si>
+  <si>
+    <t>Perty-fy</t>
+  </si>
+  <si>
+    <t>Re-factor</t>
+  </si>
+  <si>
+    <t>Make It Snazzy</t>
   </si>
 </sst>
 </file>
@@ -620,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA663AC-154D-4CA4-8714-529D6DD42399}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +652,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -794,7 +803,7 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
@@ -856,10 +865,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -872,7 +881,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J27" t="s">
         <v>18</v>
@@ -880,20 +889,20 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -910,11 +919,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CBFA37-7657-460A-93CC-3E054184B077}">
-  <dimension ref="B1:U10"/>
+  <dimension ref="B1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -923,14 +930,15 @@
     <col min="4" max="5" width="3.85546875" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="3.85546875" customWidth="1"/>
     <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="3.85546875" customWidth="1"/>
     <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="3.85546875" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="3.85546875" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -938,18 +946,21 @@
         <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -958,7 +969,7 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
@@ -972,7 +983,7 @@
       </c>
       <c r="N2" s="9"/>
       <c r="O2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="9"/>
       <c r="R2" s="7" t="s">
@@ -980,7 +991,7 @@
       </c>
       <c r="T2" s="9"/>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
@@ -988,7 +999,7 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
         <v>27</v>
       </c>
@@ -1002,11 +1013,15 @@
       </c>
       <c r="N3" s="9"/>
       <c r="O3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="9"/>
       <c r="R3" s="7" t="s">
         <v>27</v>
+      </c>
+      <c r="T3" s="9"/>
+      <c r="U3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
@@ -1014,33 +1029,33 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="8"/>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
@@ -1059,60 +1074,60 @@
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O6" s="7"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="7" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E7" s="9"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O7" s="7"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E8" s="9"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" s="7"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="7" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
@@ -1125,18 +1140,20 @@
         <v>25</v>
       </c>
       <c r="O9" s="7"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="7" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H10" s="9"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="7" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="L10" s="7"/>
       <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H11" s="9"/>
+      <c r="I11" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solo Project: Python routes
</commit_message>
<xml_diff>
--- a/solo-project.xlsx
+++ b/solo-project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tiffany\coding-dojo\projects_and_algos\solo-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A869CA71-37BC-43B6-8C16-C24263B0AD36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582CB19A-6EC3-46B2-A0D4-3D81C379BE60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>Recipes and Grocery List App</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Make It Snazzy</t>
+  </si>
+  <si>
+    <t>Step re-order (create easier process)</t>
   </si>
 </sst>
 </file>
@@ -627,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA663AC-154D-4CA4-8714-529D6DD42399}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,23 +871,23 @@
         <v>33</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="I26" t="s">
-        <v>10</v>
+      <c r="J26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>44</v>
       </c>
-      <c r="J27" t="s">
-        <v>18</v>
+      <c r="I27" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -892,16 +895,26 @@
         <v>46</v>
       </c>
       <c r="I28" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solo Project: BE Setup and FE Integration
</commit_message>
<xml_diff>
--- a/solo-project.xlsx
+++ b/solo-project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tiffany\coding-dojo\projects_and_algos\solo-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582CB19A-6EC3-46B2-A0D4-3D81C379BE60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E91AC67-FE7B-4B61-B5FC-A24672449045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overview" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>Recipes and Grocery List App</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Test Database</t>
-  </si>
-  <si>
-    <t>Back-End Setup</t>
   </si>
   <si>
     <t>Testing</t>
@@ -187,9 +184,6 @@
     <t>Delete Recipe (R Book and Modify R)</t>
   </si>
   <si>
-    <t>ORM Database (Alt)</t>
-  </si>
-  <si>
     <t>Perty-fy</t>
   </si>
   <si>
@@ -200,13 +194,124 @@
   </si>
   <si>
     <t>Step re-order (create easier process)</t>
+  </si>
+  <si>
+    <t>Setup ORM Database (Alt)</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Recipe Book</t>
+  </si>
+  <si>
+    <t>POSTs</t>
+  </si>
+  <si>
+    <t>GETs</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Session Clear</t>
+  </si>
+  <si>
+    <t>Primary Setup, From/Import, Init, Constants</t>
+  </si>
+  <si>
+    <t>Back-End Setup (MySQL)</t>
+  </si>
+  <si>
+    <t>Filtering, order by, etc</t>
+  </si>
+  <si>
+    <t>Add New Recipe</t>
+  </si>
+  <si>
+    <t>Ensure Ingredient amounts (recipes_have_ingredients) and instructions (instructions table) are deleted (but not from Ingredients table) upon Recipe deletion.</t>
+  </si>
+  <si>
+    <t>Validations</t>
+  </si>
+  <si>
+    <t>Registration Failure</t>
+  </si>
+  <si>
+    <t>Registration Success</t>
+  </si>
+  <si>
+    <t>Update Profile Failure</t>
+  </si>
+  <si>
+    <t>Update Profile Success</t>
+  </si>
+  <si>
+    <t>Update Login Info Failure</t>
+  </si>
+  <si>
+    <t>Update Login Info Success</t>
+  </si>
+  <si>
+    <t>Add Ingredient Failure</t>
+  </si>
+  <si>
+    <t>Add Recipe Failure</t>
+  </si>
+  <si>
+    <t>Add Recipe Success</t>
+  </si>
+  <si>
+    <t>Modify Recipe Failure</t>
+  </si>
+  <si>
+    <t>Modify Recipe Success</t>
+  </si>
+  <si>
+    <t>Delete Recipe Failure</t>
+  </si>
+  <si>
+    <t>Delete Recipe Success</t>
+  </si>
+  <si>
+    <t>Login Failure (need failure flash for no email match)</t>
+  </si>
+  <si>
+    <t>Add Ingredient</t>
+  </si>
+  <si>
+    <t>More refactoring/refining</t>
+  </si>
+  <si>
+    <t>Add Ingredient Success (need failure for ingredient already in master list)</t>
+  </si>
+  <si>
+    <t>Delete Steps and Ingredients on Recipe delete (cascade)</t>
+  </si>
+  <si>
+    <t>Check Recipe Add at each Insert Query - do not add  if failure at any point?</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Search functions</t>
+  </si>
+  <si>
+    <t>Egde case - if steps or ingredients not added in original Add Recipe - how to tie to recipe, or must require 1 step and 1 ingredient on add recipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +364,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +411,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -287,13 +426,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
@@ -309,15 +449,20 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA663AC-154D-4CA4-8714-529D6DD42399}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,131 +799,131 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="A6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -806,7 +951,7 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I18" t="s">
         <v>12</v>
@@ -835,8 +980,8 @@
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="I21" t="s">
-        <v>8</v>
+      <c r="J21" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -844,8 +989,8 @@
       <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="J22" t="s">
-        <v>13</v>
+      <c r="I22" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -854,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="J23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -863,59 +1008,94 @@
         <v>8</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="J25" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="J26" t="s">
-        <v>54</v>
+      <c r="I26" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>44</v>
-      </c>
-      <c r="I27" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="J27" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J29" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I30" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J31" t="s">
-        <v>45</v>
+      <c r="I31" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I32" t="s">
-        <v>36</v>
+      <c r="J32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -932,243 +1112,372 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CBFA37-7657-460A-93CC-3E054184B077}">
-  <dimension ref="B1:U11"/>
+  <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="3.85546875" customWidth="1"/>
-    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="3.85546875" customWidth="1"/>
-    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="3.85546875" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="3.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" style="7" customWidth="1"/>
+    <col min="10" max="11" width="3.85546875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" style="7" customWidth="1"/>
+    <col min="13" max="14" width="3.85546875" style="7" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="3.85546875" style="7" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.85546875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="2:21" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="3" t="s">
+      <c r="R1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" t="s">
+    <row r="2" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="K2" s="8"/>
       <c r="L2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="10"/>
       <c r="O2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="Q2" s="10"/>
       <c r="R2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="9"/>
-      <c r="U2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" t="s">
+      <c r="T2" s="10"/>
+      <c r="U2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="K3" s="8"/>
       <c r="L3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="9"/>
+      <c r="N3" s="10"/>
       <c r="O3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="9"/>
-      <c r="U3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" t="s">
+      <c r="T3" s="10"/>
+      <c r="U3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="9"/>
-      <c r="O4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="9"/>
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="K5" s="8"/>
       <c r="L5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="Q5" s="9"/>
+      <c r="O5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" s="10"/>
       <c r="R5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E6" s="8"/>
+    <row r="6" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="E6" s="9"/>
       <c r="F6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="K6" s="8"/>
       <c r="L6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="Q6" s="9"/>
+      <c r="Q6" s="10"/>
       <c r="R6" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="E7" s="9"/>
+      <c r="F7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E7" s="8"/>
-      <c r="F7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="7"/>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="10"/>
       <c r="R7" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="E8" s="8"/>
       <c r="F8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="H8" s="8"/>
       <c r="I8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="K8" s="8"/>
       <c r="L8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="7"/>
-      <c r="Q8" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="10"/>
       <c r="R8" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H9" s="9"/>
+    <row r="9" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="E9" s="9"/>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="K9" s="8"/>
       <c r="L9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="H10" s="8"/>
       <c r="I10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="H11" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="8"/>
+      <c r="O10" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="H11" s="8"/>
       <c r="I11" s="7" t="s">
-        <v>30</v>
+        <v>82</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="H12" s="8"/>
+      <c r="I12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="8"/>
+      <c r="O12" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="I13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="8"/>
+      <c r="O13" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="H14" s="9"/>
+      <c r="I14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="H15" s="9"/>
+      <c r="I15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="H16" s="8"/>
+      <c r="I16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="N16" s="8"/>
+      <c r="O16" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="H17" s="8"/>
+      <c r="I17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" s="13"/>
+      <c r="O17" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="H18" s="8"/>
+      <c r="I18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="14"/>
+      <c r="O18" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N19" s="8"/>
+      <c r="O19" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="H20" s="9"/>
+      <c r="I20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N20" s="14"/>
+      <c r="O20" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N21" s="8"/>
+      <c r="O21" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N22" s="14"/>
+      <c r="O22" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N23" s="8"/>
+      <c r="O23" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solo Project: update templates, server, flash (re)
</commit_message>
<xml_diff>
--- a/solo-project.xlsx
+++ b/solo-project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tiffany\coding-dojo\projects_and_algos\solo-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E91AC67-FE7B-4B61-B5FC-A24672449045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B9FDB-83F9-4C11-B2AD-06574C35C8CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
   <si>
     <t>Recipes and Grocery List App</t>
   </si>
@@ -181,9 +181,6 @@
     <t>Modify/Delete Recipe</t>
   </si>
   <si>
-    <t>Delete Recipe (R Book and Modify R)</t>
-  </si>
-  <si>
     <t>Perty-fy</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>Update Login Info Success</t>
   </si>
   <si>
-    <t>Add Ingredient Failure</t>
-  </si>
-  <si>
     <t>Add Recipe Failure</t>
   </si>
   <si>
@@ -283,15 +277,9 @@
     <t>Login Failure (need failure flash for no email match)</t>
   </si>
   <si>
-    <t>Add Ingredient</t>
-  </si>
-  <si>
     <t>More refactoring/refining</t>
   </si>
   <si>
-    <t>Add Ingredient Success (need failure for ingredient already in master list)</t>
-  </si>
-  <si>
     <t>Delete Steps and Ingredients on Recipe delete (cascade)</t>
   </si>
   <si>
@@ -305,6 +293,51 @@
   </si>
   <si>
     <t>Egde case - if steps or ingredients not added in original Add Recipe - how to tie to recipe, or must require 1 step and 1 ingredient on add recipe</t>
+  </si>
+  <si>
+    <t>Delete Recipe (Update Recipe)</t>
+  </si>
+  <si>
+    <t>Delete Recipe (Recipe Book)</t>
+  </si>
+  <si>
+    <t>View/Modify Recipe</t>
+  </si>
+  <si>
+    <t>View Recipe (Main section)</t>
+  </si>
+  <si>
+    <t>View Recipe (Ingredients)</t>
+  </si>
+  <si>
+    <t>View Recipe (Instructions)</t>
+  </si>
+  <si>
+    <t>Future or Unused</t>
+  </si>
+  <si>
+    <t>Add Master Ingredient</t>
+  </si>
+  <si>
+    <t>Add Master Ingredient Success</t>
+  </si>
+  <si>
+    <t>View Recipe (Directions)</t>
+  </si>
+  <si>
+    <t>Add Recipe Ingredient Failure</t>
+  </si>
+  <si>
+    <t>Add Recipe Instruction Failure</t>
+  </si>
+  <si>
+    <t>Add Master Ingredient Failure</t>
+  </si>
+  <si>
+    <t>View Recipe (Add Ingredients)</t>
+  </si>
+  <si>
+    <t>View Recipe (Add Directions)</t>
   </si>
 </sst>
 </file>
@@ -452,11 +485,11 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -799,131 +832,131 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -981,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1032,7 +1065,7 @@
         <v>43</v>
       </c>
       <c r="J27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1070,32 +1103,32 @@
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1112,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CBFA37-7657-460A-93CC-3E054184B077}">
-  <dimension ref="B1:U23"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1178,7 @@
         <v>46</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>23</v>
@@ -1154,7 +1187,7 @@
         <v>31</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U1" s="11" t="s">
         <v>28</v>
@@ -1171,7 +1204,7 @@
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="7" t="s">
@@ -1187,7 +1220,7 @@
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="15" x14ac:dyDescent="0.25">
@@ -1201,7 +1234,7 @@
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="7" t="s">
@@ -1217,7 +1250,7 @@
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:21" ht="15" x14ac:dyDescent="0.25">
@@ -1230,7 +1263,7 @@
         <v>41</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="7" t="s">
@@ -1252,18 +1285,18 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="7" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="7" t="s">
@@ -1271,17 +1304,17 @@
       </c>
     </row>
     <row r="6" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="E6" s="9"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="7" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="7" t="s">
@@ -1289,36 +1322,36 @@
       </c>
     </row>
     <row r="7" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="E7" s="9"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="7" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="K7" s="13"/>
       <c r="L7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="7" t="s">
-        <v>40</v>
+        <v>99</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="E8" s="8"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="7" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="K8" s="13"/>
       <c r="L8" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="N8" s="13"/>
       <c r="O8" s="7" t="s">
         <v>67</v>
       </c>
@@ -1328,9 +1361,9 @@
       </c>
     </row>
     <row r="9" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="E9" s="9"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="7" t="s">
@@ -1338,9 +1371,9 @@
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="N9" s="8"/>
+        <v>86</v>
+      </c>
+      <c r="N9" s="13"/>
       <c r="O9" s="7" t="s">
         <v>68</v>
       </c>
@@ -1348,66 +1381,77 @@
     <row r="10" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="H10" s="8"/>
       <c r="I10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="K10" s="13"/>
       <c r="L10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="H11" s="8"/>
-      <c r="I11" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="7" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="H12" s="8"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="8"/>
+        <v>59</v>
+      </c>
+      <c r="N12" s="13"/>
       <c r="O12" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="H13" s="9"/>
       <c r="I13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N13" s="8"/>
+        <v>58</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="13"/>
       <c r="O13" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="H14" s="9"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" s="13"/>
       <c r="O14" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="H15" s="9"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N15" s="8"/>
+        <v>89</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" s="13"/>
       <c r="O15" s="7" t="s">
         <v>73</v>
       </c>
@@ -1415,65 +1459,184 @@
     <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="H16" s="8"/>
       <c r="I16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="N16" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="L16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="13"/>
       <c r="O16" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="H17" s="8"/>
       <c r="I17" s="7" t="s">
-        <v>29</v>
+        <v>95</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="N17" s="13"/>
       <c r="O17" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="8:15" ht="15" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="H18" s="8"/>
       <c r="I18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="14"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" s="13"/>
       <c r="O18" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K19" s="8"/>
+      <c r="L19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K20" s="8"/>
+      <c r="L20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N20" s="13"/>
+      <c r="O20" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K21" s="8"/>
+      <c r="L21" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K22" s="8"/>
+      <c r="L22" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K23" s="13"/>
+      <c r="L23" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K24" s="8"/>
+      <c r="L24" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K25" s="8"/>
+      <c r="L25" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="K26" s="8"/>
+      <c r="L26" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="E33" s="9"/>
+      <c r="F33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="8"/>
+      <c r="I33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="8"/>
+      <c r="L33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="E34" s="8"/>
+      <c r="F34" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="L34" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E35" s="9"/>
+      <c r="F35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K35" s="10"/>
+      <c r="L35" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="H36" s="8"/>
+      <c r="I36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K36" s="8"/>
+      <c r="L36" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="K37" s="13"/>
+      <c r="L37" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="K38" s="13"/>
+      <c r="L38" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="K39" s="13"/>
+      <c r="L39" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="8:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="N19" s="8"/>
-      <c r="O19" s="7" t="s">
+    <row r="40" spans="5:18" ht="15" x14ac:dyDescent="0.25">
+      <c r="K40" s="13"/>
+      <c r="L40" s="7" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="8:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="H20" s="9"/>
-      <c r="I20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="N20" s="14"/>
-      <c r="O20" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="8:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="N21" s="8"/>
-      <c r="O21" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="8:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="N22" s="14"/>
-      <c r="O22" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="8:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="N23" s="8"/>
-      <c r="O23" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Styling: updated all pages
</commit_message>
<xml_diff>
--- a/solo-project.xlsx
+++ b/solo-project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tiffany\coding-dojo\projects_and_algos\solo-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B9FDB-83F9-4C11-B2AD-06574C35C8CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4598DC69-1950-4F1E-93D7-B25532043F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6F34D44-09B2-4C36-9E56-DCADF960275C}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overview" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="103">
   <si>
     <t>Recipes and Grocery List App</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>View Recipe (Add Directions)</t>
+  </si>
+  <si>
+    <t>User Session Check - all pages</t>
+  </si>
+  <si>
+    <t>Allow for user to update images</t>
   </si>
 </sst>
 </file>
@@ -808,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA663AC-154D-4CA4-8714-529D6DD42399}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,6 +1135,16 @@
     <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CBFA37-7657-460A-93CC-3E054184B077}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>

</xml_diff>